<commit_message>
Add smooth transition for sidebar and main content area; remove hamburger menu oval effect
</commit_message>
<xml_diff>
--- a/frontend/noti.xlsx
+++ b/frontend/noti.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Go Live</t>
+          <t>Not Started</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Go Live</t>
+          <t>Not Started</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 'web' column to Biller model, update migration, and include web URLs in API responses
</commit_message>
<xml_diff>
--- a/frontend/noti.xlsx
+++ b/frontend/noti.xlsx
@@ -514,7 +514,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Go Live</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Go Live</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Go Live</t>
         </is>
       </c>
     </row>

</xml_diff>